<commit_message>
fix: change canonical url in build
</commit_message>
<xml_diff>
--- a/output/CodeSystem-OsirisCS.xlsx
+++ b/output/CodeSystem-OsirisCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="452">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-16T15:52:24+01:00</t>
+    <t>2023-03-28T11:28:20+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -111,7 +111,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>105</t>
+    <t>206</t>
   </si>
   <si>
     <t>Level</t>
@@ -772,6 +772,603 @@
   </si>
   <si>
     <t>O6-OTH</t>
+  </si>
+  <si>
+    <t>O13-OTH</t>
+  </si>
+  <si>
+    <t>O7-1</t>
+  </si>
+  <si>
+    <t>Affymetrix Cytoscan HD</t>
+  </si>
+  <si>
+    <t>O7-2</t>
+  </si>
+  <si>
+    <t>Affymetrix EMET Plus Premier Pack</t>
+  </si>
+  <si>
+    <t>O7-3</t>
+  </si>
+  <si>
+    <t>Affymetrix Genome-Wide Human SNP Array 5.0</t>
+  </si>
+  <si>
+    <t>O7-4</t>
+  </si>
+  <si>
+    <t>Affymetrix Genome-Wide Human SNP Array 6.0</t>
+  </si>
+  <si>
+    <t>O7-5</t>
+  </si>
+  <si>
+    <t>Affymetrix HT Human Genome U133A Array Plate Set</t>
+  </si>
+  <si>
+    <t>O7-6</t>
+  </si>
+  <si>
+    <t>Affymetrix Human Exon 1.0 ST</t>
+  </si>
+  <si>
+    <t>O7-7</t>
+  </si>
+  <si>
+    <t>Affymetrix Human Gene 1.0 ST</t>
+  </si>
+  <si>
+    <t>O7-8</t>
+  </si>
+  <si>
+    <t>Affymetrix Human Genome U219 Array Plate</t>
+  </si>
+  <si>
+    <t>O7-9</t>
+  </si>
+  <si>
+    <t>Affymetrix Human MIP 330K</t>
+  </si>
+  <si>
+    <t>O7-10</t>
+  </si>
+  <si>
+    <t>Affymetrix Human U133 Plus 2.0</t>
+  </si>
+  <si>
+    <t>O7-11</t>
+  </si>
+  <si>
+    <t>Affymetrix Human U133 Plus PM</t>
+  </si>
+  <si>
+    <t>O7-12</t>
+  </si>
+  <si>
+    <t>Affymetrix Mapping 100K Array Set</t>
+  </si>
+  <si>
+    <t>O7-13</t>
+  </si>
+  <si>
+    <t>Affymetrix Mapping 10K 2.0 Array Set</t>
+  </si>
+  <si>
+    <t>O7-14</t>
+  </si>
+  <si>
+    <t>Affymetrix Mapping 500K Array Set</t>
+  </si>
+  <si>
+    <t>O7-15</t>
+  </si>
+  <si>
+    <t>Affymetrix OncoScan FFPE Express 2.0</t>
+  </si>
+  <si>
+    <t>O7-16</t>
+  </si>
+  <si>
+    <t>Agilent 244K Custom Gene Expression G4502A-07</t>
+  </si>
+  <si>
+    <t>O7-17</t>
+  </si>
+  <si>
+    <t>Agilent 244K Custom Gene Expression G4502A-07-1</t>
+  </si>
+  <si>
+    <t>O7-18</t>
+  </si>
+  <si>
+    <t>Agilent 244K Custom Gene Expression G4502A-07-2</t>
+  </si>
+  <si>
+    <t>O7-19</t>
+  </si>
+  <si>
+    <t>Agilent 244K Custom Gene Expression G4502A-07-3</t>
+  </si>
+  <si>
+    <t>O7-20</t>
+  </si>
+  <si>
+    <t>Agilent 8 x 15K Human miRNA-specific microarray</t>
+  </si>
+  <si>
+    <t>O7-21</t>
+  </si>
+  <si>
+    <t>Agilent Human CGH 1x1M</t>
+  </si>
+  <si>
+    <t>O7-22</t>
+  </si>
+  <si>
+    <t>Agilent Human CGH 2x400K</t>
+  </si>
+  <si>
+    <t>O7-23</t>
+  </si>
+  <si>
+    <t>Agilent Human CGH 4x180K</t>
+  </si>
+  <si>
+    <t>O7-24</t>
+  </si>
+  <si>
+    <t>Agilent Human CGH 8x60K</t>
+  </si>
+  <si>
+    <t>O7-25</t>
+  </si>
+  <si>
+    <t>Agilent Human CNV 2x400K</t>
+  </si>
+  <si>
+    <t>O7-26</t>
+  </si>
+  <si>
+    <t>Agilent Human CNV Association 2x105K</t>
+  </si>
+  <si>
+    <t>O7-27</t>
+  </si>
+  <si>
+    <t>Agilent Human CpG Island Microarray Kit</t>
+  </si>
+  <si>
+    <t>O7-28</t>
+  </si>
+  <si>
+    <t>Agilent Human Genome 105A</t>
+  </si>
+  <si>
+    <t>O7-29</t>
+  </si>
+  <si>
+    <t>Agilent Human Genome 244A</t>
+  </si>
+  <si>
+    <t>O7-30</t>
+  </si>
+  <si>
+    <t>Agilent Human Genome 44K</t>
+  </si>
+  <si>
+    <t>O7-31</t>
+  </si>
+  <si>
+    <t>Agilent Human Genome CGH Custom Microaary 2x415K</t>
+  </si>
+  <si>
+    <t>O7-32</t>
+  </si>
+  <si>
+    <t>Agilent Human miRNA Microarray Kit (v2)</t>
+  </si>
+  <si>
+    <t>O7-33</t>
+  </si>
+  <si>
+    <t>Agilent Human Promoter ChIP-on-chip Microarray Set</t>
+  </si>
+  <si>
+    <t>O7-34</t>
+  </si>
+  <si>
+    <t>Agilent Human SpliceArray</t>
+  </si>
+  <si>
+    <t>O7-35</t>
+  </si>
+  <si>
+    <t>Agilent Whole Human Genome Oligo Microarray Kit</t>
+  </si>
+  <si>
+    <t>O7-36</t>
+  </si>
+  <si>
+    <t>Almac Human CRC</t>
+  </si>
+  <si>
+    <t>O7-37</t>
+  </si>
+  <si>
+    <t>capillary sequencing</t>
+  </si>
+  <si>
+    <t>O7-38</t>
+  </si>
+  <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>O7-39</t>
+  </si>
+  <si>
+    <t>Custom-designed cDNA array</t>
+  </si>
+  <si>
+    <t>O7-40</t>
+  </si>
+  <si>
+    <t>Custom-designed gene expression array</t>
+  </si>
+  <si>
+    <t>O7-41</t>
+  </si>
+  <si>
+    <t>Helicos sequencing</t>
+  </si>
+  <si>
+    <t>O7-42</t>
+  </si>
+  <si>
+    <t>HumanOmni2.5-8 BeadChip Kit</t>
+  </si>
+  <si>
+    <t>O7-43</t>
+  </si>
+  <si>
+    <t>Illumina GA sequencing</t>
+  </si>
+  <si>
+    <t>O7-44</t>
+  </si>
+  <si>
+    <t>Illumina goldengate methylation</t>
+  </si>
+  <si>
+    <t>O7-45</t>
+  </si>
+  <si>
+    <t>Illumina GoldenGate Methylation Cancer Panel I</t>
+  </si>
+  <si>
+    <t>O7-46</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq</t>
+  </si>
+  <si>
+    <t>O7-47</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq X Ten</t>
+  </si>
+  <si>
+    <t>O7-48</t>
+  </si>
+  <si>
+    <t>Illumina Human Omni1-Quad beadchip</t>
+  </si>
+  <si>
+    <t>O7-49</t>
+  </si>
+  <si>
+    <t>Illumina Human1M OmniQuad chip</t>
+  </si>
+  <si>
+    <t>O7-50</t>
+  </si>
+  <si>
+    <t>Illumina human1m-duo</t>
+  </si>
+  <si>
+    <t>O7-51</t>
+  </si>
+  <si>
+    <t>Illumina human510s-duo</t>
+  </si>
+  <si>
+    <t>O7-52</t>
+  </si>
+  <si>
+    <t>Illumina human660w-quad</t>
+  </si>
+  <si>
+    <t>O7-53</t>
+  </si>
+  <si>
+    <t>Illumina HumanCNV370-Duo v1.0 BeadChip</t>
+  </si>
+  <si>
+    <t>O7-54</t>
+  </si>
+  <si>
+    <t>Illumina humancytosnp-12</t>
+  </si>
+  <si>
+    <t>O7-55</t>
+  </si>
+  <si>
+    <t>Illumina HumanHap550</t>
+  </si>
+  <si>
+    <t>O7-56</t>
+  </si>
+  <si>
+    <t>Illumina HumanHT-12 v4.0 beadchip</t>
+  </si>
+  <si>
+    <t>O7-57</t>
+  </si>
+  <si>
+    <t>Illumina humanht-16</t>
+  </si>
+  <si>
+    <t>O7-58</t>
+  </si>
+  <si>
+    <t>Illumina humanht-17</t>
+  </si>
+  <si>
+    <t>O7-59</t>
+  </si>
+  <si>
+    <t>Illumina humanmethylation27</t>
+  </si>
+  <si>
+    <t>O7-60</t>
+  </si>
+  <si>
+    <t>Illumina HumanOmniExpress BeadChip</t>
+  </si>
+  <si>
+    <t>O7-61</t>
+  </si>
+  <si>
+    <t>Illumina HumanRef-8 v3.0 beadchip</t>
+  </si>
+  <si>
+    <t>O7-62</t>
+  </si>
+  <si>
+    <t>Illumina HumanWG-6 v3.0 beadchip</t>
+  </si>
+  <si>
+    <t>O7-63</t>
+  </si>
+  <si>
+    <t>Illumina Infinium HumanMethylation450</t>
+  </si>
+  <si>
+    <t>O7-64</t>
+  </si>
+  <si>
+    <t>Illumina microRNA Expression Profiling Panel</t>
+  </si>
+  <si>
+    <t>O7-65</t>
+  </si>
+  <si>
+    <t>Illumina MiSeq Personal Sequencer</t>
+  </si>
+  <si>
+    <t>O7-66</t>
+  </si>
+  <si>
+    <t>Ion Torrent PGM</t>
+  </si>
+  <si>
+    <t>O7-67</t>
+  </si>
+  <si>
+    <t>Ion Torrent Proton</t>
+  </si>
+  <si>
+    <t>O7-68</t>
+  </si>
+  <si>
+    <t>M.D. Anderson Reverse Phase Protein Array Core</t>
+  </si>
+  <si>
+    <t>O7-69</t>
+  </si>
+  <si>
+    <t>Microsatellite Instability Analysis</t>
+  </si>
+  <si>
+    <t>O7-70</t>
+  </si>
+  <si>
+    <t>nanoString</t>
+  </si>
+  <si>
+    <t>O7-71</t>
+  </si>
+  <si>
+    <t>Nimblegen CGS</t>
+  </si>
+  <si>
+    <t>O7-72</t>
+  </si>
+  <si>
+    <t>Nimblegen Gene Expression 12x135K</t>
+  </si>
+  <si>
+    <t>O7-73</t>
+  </si>
+  <si>
+    <t>Nimblegen Gene Expression 385K</t>
+  </si>
+  <si>
+    <t>O7-74</t>
+  </si>
+  <si>
+    <t>Nimblegen Gene Expression 4x72K</t>
+  </si>
+  <si>
+    <t>O7-75</t>
+  </si>
+  <si>
+    <t>Nimblegen Human CGH 2.1M Whole-Genome v2.0D Array</t>
+  </si>
+  <si>
+    <t>O7-76</t>
+  </si>
+  <si>
+    <t>Nimblegen Human CGH 3x720 Whole-Genome v3.0 Array</t>
+  </si>
+  <si>
+    <t>O7-77</t>
+  </si>
+  <si>
+    <t>Nimblegen Human Methylation 2.1M Whole-Genome sets</t>
+  </si>
+  <si>
+    <t>O7-78</t>
+  </si>
+  <si>
+    <t>Nimblegen Human Methylation 385K Whole-Genome sets</t>
+  </si>
+  <si>
+    <t>O7-79</t>
+  </si>
+  <si>
+    <t>PacBio RS sequencing</t>
+  </si>
+  <si>
+    <t>O7-80</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>O7-81</t>
+  </si>
+  <si>
+    <t>PCR and capillary sequencing</t>
+  </si>
+  <si>
+    <t>O7-82</t>
+  </si>
+  <si>
+    <t>qPCR</t>
+  </si>
+  <si>
+    <t>O7-83</t>
+  </si>
+  <si>
+    <t>Roche 454 sequencing</t>
+  </si>
+  <si>
+    <t>O7-84</t>
+  </si>
+  <si>
+    <t>Sequenom MassARRAY</t>
+  </si>
+  <si>
+    <t>O7-85</t>
+  </si>
+  <si>
+    <t>SOLiD sequencing</t>
+  </si>
+  <si>
+    <t>O7-86</t>
+  </si>
+  <si>
+    <t>Digital PCR</t>
+  </si>
+  <si>
+    <t>O7-87</t>
+  </si>
+  <si>
+    <t>NextSeq 500</t>
+  </si>
+  <si>
+    <t>O7-88</t>
+  </si>
+  <si>
+    <t>NovaSeq</t>
+  </si>
+  <si>
+    <t>O7-OTH</t>
+  </si>
+  <si>
+    <t>O10-1</t>
+  </si>
+  <si>
+    <t>Ion AmpliSeq Cancer Hotspot Panel v2</t>
+  </si>
+  <si>
+    <t>O10-2</t>
+  </si>
+  <si>
+    <t>Ion AmpliSeq Colon and Lung Cancer Research Panel v2</t>
+  </si>
+  <si>
+    <t>O10-3</t>
+  </si>
+  <si>
+    <t>Ion AmpliSeq Comprehensive Cancer Panel</t>
+  </si>
+  <si>
+    <t>O10-4</t>
+  </si>
+  <si>
+    <t>Ion AmpliSeq Oncomine Comprehensive Assay</t>
+  </si>
+  <si>
+    <t>O10-5</t>
+  </si>
+  <si>
+    <t>Ion AmpliSeq Oncomine Focus Assay</t>
+  </si>
+  <si>
+    <t>O10-6</t>
+  </si>
+  <si>
+    <t>Ion AmpliSeq TP53 Research Panel</t>
+  </si>
+  <si>
+    <t>O10-7</t>
+  </si>
+  <si>
+    <t>Lyric: Ion AmpliSeq Profiler</t>
+  </si>
+  <si>
+    <t>O10-8</t>
+  </si>
+  <si>
+    <t>QIAGEN GeneRead DNAseq Targeted Panels V2</t>
+  </si>
+  <si>
+    <t>O10-9</t>
+  </si>
+  <si>
+    <t>SAFIR02 Panel</t>
+  </si>
+  <si>
+    <t>O10-10</t>
+  </si>
+  <si>
+    <t>Mosc3</t>
+  </si>
+  <si>
+    <t>010-OTH</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1677,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D207"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2570,6 +3167,1220 @@
         <v>250</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B107" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="C107" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="D107" t="s" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B108" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="C108" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B109" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="C109" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B110" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="C110" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B111" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="C111" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B112" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="C112" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B113" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="C113" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B114" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="C114" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B115" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="C115" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B116" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="C116" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B117" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="C117" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B118" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="C118" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B119" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="C119" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B120" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="C120" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B121" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="C121" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B122" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="C122" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B123" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="C123" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B124" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="C124" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B125" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="C125" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B126" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="C126" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B127" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="C127" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B128" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="C128" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B129" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="C129" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B130" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="C130" t="s" s="2">
+        <v>299</v>
+      </c>
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B131" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="C131" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="D131" s="2"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B132" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="C132" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B133" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="C133" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="D133" s="2"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B134" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="C134" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="D134" s="2"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B135" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="C135" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B136" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="C136" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B137" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="C137" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B138" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="C138" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B139" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="C139" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B140" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="C140" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B141" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="C141" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B142" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="C142" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B143" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="C143" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B144" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="C144" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B145" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="C145" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="D145" s="2"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B146" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="C146" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="D146" s="2"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B147" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="C147" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="D147" s="2"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B148" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="C148" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B149" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="C149" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="D149" s="2"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B150" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="C150" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B151" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="C151" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="D151" s="2"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B152" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="C152" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B153" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="C153" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="D153" s="2"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B154" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="C154" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="D154" s="2"/>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B155" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="C155" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="D155" s="2"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B156" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="C156" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="D156" s="2"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B157" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="C157" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="D157" s="2"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B158" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="C158" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="D158" s="2"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B159" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="C159" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="D159" s="2"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B160" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="C160" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="D160" s="2"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B161" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="C161" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="D161" s="2"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B162" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="C162" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="D162" s="2"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B163" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="C163" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="D163" s="2"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B164" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="C164" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="D164" s="2"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B165" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="C165" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="D165" s="2"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B166" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="C166" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="D166" s="2"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B167" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="C167" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="D167" s="2"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B168" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="C168" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="D168" s="2"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B169" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="C169" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="D169" s="2"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B170" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="C170" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="D170" s="2"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B171" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="C171" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="D171" s="2"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B172" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="C172" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="D172" s="2"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B173" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="C173" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="D173" s="2"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B174" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="C174" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="D174" s="2"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B175" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="C175" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="D175" s="2"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B176" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="C176" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="D176" s="2"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B177" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="C177" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="D177" s="2"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B178" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="C178" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="D178" s="2"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B179" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="C179" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="D179" s="2"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B180" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="C180" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B181" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="C181" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="D181" s="2"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B182" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="C182" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="D182" s="2"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B183" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="C183" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="D183" s="2"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B184" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="C184" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="D184" s="2"/>
+    </row>
+    <row r="185">
+      <c r="A185" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B185" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="C185" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="D185" s="2"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B186" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="C186" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B187" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="C187" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="D187" s="2"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B188" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="C188" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="D188" s="2"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B189" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="C189" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="D189" s="2"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B190" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="C190" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="D190" s="2"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B191" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="C191" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="D191" s="2"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B192" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="C192" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="D192" s="2"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B193" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="C193" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="D193" s="2"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B194" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="C194" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="D194" s="2"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B195" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="C195" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="D195" s="2"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B196" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="C196" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="D196" s="2"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B197" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="C197" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="D197" s="2"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B198" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="C198" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B199" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="C199" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="D199" s="2"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B200" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="C200" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B201" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="C201" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="D201" s="2"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B202" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="C202" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="D202" s="2"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B203" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="C203" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="D203" s="2"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B204" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="C204" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="D204" s="2"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B205" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="C205" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="D205" s="2"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B206" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="C206" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="D206" s="2"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B207" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="C207" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="D207" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>